<commit_message>
fix constraint and add violation note
</commit_message>
<xml_diff>
--- a/src/data_uisi.xlsx
+++ b/src/data_uisi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acern\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978290B9-F7AD-4EA9-9984-DA1E24C97F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E8D1A3-6025-4180-808E-842976C7C9B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{35A121DA-9B65-45CA-BEBF-895C36E667B5}"/>
   </bookViews>
@@ -5158,8 +5158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84397B3-03F7-4516-8818-17F518B1BA4E}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="E98" sqref="E98"/>
+    <sheetView tabSelected="1" topLeftCell="B50" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5216,7 +5216,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -5236,7 +5236,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -5256,7 +5256,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -5276,7 +5276,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -5299,7 +5299,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -5322,7 +5322,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -5345,7 +5345,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -5368,7 +5368,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -5391,7 +5391,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -5414,7 +5414,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -5437,7 +5437,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -5460,7 +5460,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -5483,7 +5483,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -5506,7 +5506,7 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -5529,7 +5529,7 @@
         <v>0</v>
       </c>
       <c r="G16">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -5552,7 +5552,7 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -5575,7 +5575,7 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -5598,7 +5598,7 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -5621,7 +5621,7 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -5644,7 +5644,7 @@
         <v>0</v>
       </c>
       <c r="G21">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -5667,7 +5667,7 @@
         <v>0</v>
       </c>
       <c r="G22">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -5690,7 +5690,7 @@
         <v>0</v>
       </c>
       <c r="G23">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -5713,7 +5713,7 @@
         <v>0</v>
       </c>
       <c r="G24">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -5736,7 +5736,7 @@
         <v>0</v>
       </c>
       <c r="G25">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -5759,7 +5759,7 @@
         <v>0</v>
       </c>
       <c r="G26">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -5782,7 +5782,7 @@
         <v>0</v>
       </c>
       <c r="G27">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -5805,7 +5805,7 @@
         <v>0</v>
       </c>
       <c r="G28">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -5828,7 +5828,7 @@
         <v>0</v>
       </c>
       <c r="G29">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -5851,7 +5851,7 @@
         <v>0</v>
       </c>
       <c r="G30">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -5874,7 +5874,7 @@
         <v>0</v>
       </c>
       <c r="G31">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -5897,7 +5897,7 @@
         <v>0</v>
       </c>
       <c r="G32">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -5920,7 +5920,7 @@
         <v>0</v>
       </c>
       <c r="G33">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -5943,7 +5943,7 @@
         <v>0</v>
       </c>
       <c r="G34">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -5966,7 +5966,7 @@
         <v>0</v>
       </c>
       <c r="G35">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -5989,7 +5989,7 @@
         <v>0</v>
       </c>
       <c r="G36">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -6012,7 +6012,7 @@
         <v>0</v>
       </c>
       <c r="G37">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -6035,7 +6035,7 @@
         <v>0</v>
       </c>
       <c r="G38">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -6058,7 +6058,7 @@
         <v>0</v>
       </c>
       <c r="G39">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -6081,7 +6081,7 @@
         <v>0</v>
       </c>
       <c r="G40">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -6104,7 +6104,7 @@
         <v>0</v>
       </c>
       <c r="G41">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -6127,7 +6127,7 @@
         <v>0</v>
       </c>
       <c r="G42">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -6150,7 +6150,7 @@
         <v>0</v>
       </c>
       <c r="G43">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -6173,7 +6173,7 @@
         <v>0</v>
       </c>
       <c r="G44">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -6196,7 +6196,7 @@
         <v>0</v>
       </c>
       <c r="G45">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -6219,7 +6219,7 @@
         <v>0</v>
       </c>
       <c r="G46">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -6242,7 +6242,7 @@
         <v>0</v>
       </c>
       <c r="G47">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -6265,7 +6265,7 @@
         <v>0</v>
       </c>
       <c r="G48">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -6288,7 +6288,7 @@
         <v>0</v>
       </c>
       <c r="G49">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -6311,7 +6311,7 @@
         <v>0</v>
       </c>
       <c r="G50">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -6334,7 +6334,7 @@
         <v>0</v>
       </c>
       <c r="G51">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -6357,7 +6357,7 @@
         <v>0</v>
       </c>
       <c r="G52">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -6380,7 +6380,7 @@
         <v>0</v>
       </c>
       <c r="G53">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -6403,7 +6403,7 @@
         <v>0</v>
       </c>
       <c r="G54">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -6426,7 +6426,7 @@
         <v>0</v>
       </c>
       <c r="G55">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -6449,7 +6449,7 @@
         <v>0</v>
       </c>
       <c r="G56">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -6472,7 +6472,7 @@
         <v>0</v>
       </c>
       <c r="G57">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -6495,7 +6495,7 @@
         <v>0</v>
       </c>
       <c r="G58">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -6518,7 +6518,7 @@
         <v>0</v>
       </c>
       <c r="G59">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -6541,7 +6541,7 @@
         <v>0</v>
       </c>
       <c r="G60">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -6564,7 +6564,7 @@
         <v>0</v>
       </c>
       <c r="G61">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -6587,7 +6587,7 @@
         <v>0</v>
       </c>
       <c r="G62">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -6610,7 +6610,7 @@
         <v>0</v>
       </c>
       <c r="G63">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -6633,7 +6633,7 @@
         <v>0</v>
       </c>
       <c r="G64">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -6656,7 +6656,7 @@
         <v>0</v>
       </c>
       <c r="G65">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -6679,7 +6679,7 @@
         <v>0</v>
       </c>
       <c r="G66">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -6702,7 +6702,7 @@
         <v>0</v>
       </c>
       <c r="G67">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -6725,7 +6725,7 @@
         <v>0</v>
       </c>
       <c r="G68">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -6748,7 +6748,7 @@
         <v>0</v>
       </c>
       <c r="G69">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -6771,7 +6771,7 @@
         <v>0</v>
       </c>
       <c r="G70">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -6794,7 +6794,7 @@
         <v>0</v>
       </c>
       <c r="G71">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -6804,7 +6804,7 @@
       <c r="B72" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" s="7" t="s">
         <v>231</v>
       </c>
       <c r="D72" t="s">
@@ -6814,10 +6814,10 @@
         <v>298</v>
       </c>
       <c r="F72">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G72">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -6840,7 +6840,7 @@
         <v>0</v>
       </c>
       <c r="G73">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -6863,7 +6863,7 @@
         <v>0</v>
       </c>
       <c r="G74">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -6886,7 +6886,7 @@
         <v>0</v>
       </c>
       <c r="G75">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -6909,7 +6909,7 @@
         <v>0</v>
       </c>
       <c r="G76">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -6932,7 +6932,7 @@
         <v>0</v>
       </c>
       <c r="G77">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -6942,7 +6942,7 @@
       <c r="B78" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" s="7" t="s">
         <v>237</v>
       </c>
       <c r="D78" t="s">
@@ -6952,10 +6952,10 @@
         <v>299</v>
       </c>
       <c r="F78">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G78">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H78" t="s">
         <v>302</v>
@@ -6981,7 +6981,7 @@
         <v>0</v>
       </c>
       <c r="G79">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -7004,7 +7004,7 @@
         <v>0</v>
       </c>
       <c r="G80">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -7027,7 +7027,7 @@
         <v>0</v>
       </c>
       <c r="G81">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -7050,7 +7050,7 @@
         <v>0</v>
       </c>
       <c r="G82">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -7073,7 +7073,7 @@
         <v>0</v>
       </c>
       <c r="G83">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -7096,7 +7096,7 @@
         <v>0</v>
       </c>
       <c r="G84">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -7119,7 +7119,7 @@
         <v>0</v>
       </c>
       <c r="G85">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -7139,7 +7139,7 @@
         <v>0</v>
       </c>
       <c r="G86">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -7159,7 +7159,7 @@
         <v>0</v>
       </c>
       <c r="G87">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -7179,7 +7179,7 @@
         <v>0</v>
       </c>
       <c r="G88">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -7199,7 +7199,7 @@
         <v>0</v>
       </c>
       <c r="G89">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -7219,7 +7219,7 @@
         <v>0</v>
       </c>
       <c r="G90">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -7239,7 +7239,7 @@
         <v>0</v>
       </c>
       <c r="G91">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -7259,7 +7259,7 @@
         <v>0</v>
       </c>
       <c r="G92">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -7279,7 +7279,7 @@
         <v>0</v>
       </c>
       <c r="G93">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -7299,7 +7299,7 @@
         <v>0</v>
       </c>
       <c r="G94">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -7319,7 +7319,7 @@
         <v>0</v>
       </c>
       <c r="G95">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -7339,7 +7339,7 @@
         <v>0</v>
       </c>
       <c r="G96">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -7359,7 +7359,7 @@
         <v>0</v>
       </c>
       <c r="G97">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -7379,7 +7379,7 @@
         <v>0</v>
       </c>
       <c r="G98">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -7399,7 +7399,7 @@
         <v>0</v>
       </c>
       <c r="G99">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -7419,7 +7419,7 @@
         <v>0</v>
       </c>
       <c r="G100">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>